<commit_message>
updated EDA with sample data file
</commit_message>
<xml_diff>
--- a/capstone/project_data/data_dictionary.xlsx
+++ b/capstone/project_data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thermofisher-my.sharepoint.com/personal/dengbo_yang_thermofisher_com/Documents/DS/DSproj/ds-intermediate-2023/capstone/project_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{E44779EC-5EB6-8847-A5D1-572CFCB7F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C87C3F6F-4684-4F79-B396-87495E91BAC2}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{E44779EC-5EB6-8847-A5D1-572CFCB7F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4BBE6CB-1976-40DC-8813-4C37B1FE9ABA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,9 +547,6 @@
     <t>verified_status_joint</t>
   </si>
   <si>
-    <t>The self-reported annual income provided by the borrower during registration.</t>
-  </si>
-  <si>
     <t>The upper boundary range the borrower’s FICO at loan origination belongs to.</t>
   </si>
   <si>
@@ -959,6 +956,9 @@
   </si>
   <si>
     <t>Indicates if the co-borrowers' joint income was verified by bank, not verified, or if the income source was verified</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -1994,9 +1994,9 @@
   </sheetPr>
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>49</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>50</v>
@@ -2044,10 +2044,10 @@
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -2056,7 +2056,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>171</v>
+        <v>304</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2065,7 +2065,7 @@
         <v>168</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>51</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>52</v>
@@ -2134,28 +2134,28 @@
     </row>
     <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>54</v>
@@ -2188,10 +2188,10 @@
     </row>
     <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -2200,7 +2200,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -2209,7 +2209,7 @@
         <v>169</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -2245,7 +2245,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -2254,7 +2254,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -2281,61 +2281,61 @@
         <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C37" s="5"/>
       <c r="I37" s="10"/>
@@ -2343,55 +2343,55 @@
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D43" s="4"/>
     </row>
@@ -2400,7 +2400,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D44" s="4"/>
     </row>
@@ -2409,16 +2409,16 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>190</v>
       </c>
       <c r="D46" s="4"/>
       <c r="I46" s="10"/>
@@ -2439,10 +2439,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="D48" s="4"/>
       <c r="I48" s="12"/>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="D49" s="4"/>
     </row>
@@ -2463,7 +2463,7 @@
         <v>26</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D50" s="4"/>
     </row>
@@ -2499,7 +2499,7 @@
         <v>45</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D54" s="4"/>
     </row>
@@ -2508,7 +2508,7 @@
         <v>46</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D55" s="4"/>
     </row>
@@ -2517,7 +2517,7 @@
         <v>47</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D56" s="4"/>
     </row>
@@ -2559,10 +2559,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>196</v>
       </c>
       <c r="D61" s="4"/>
     </row>
@@ -2571,12 +2571,12 @@
         <v>1</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>120</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>60</v>
@@ -2640,15 +2640,15 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>64</v>
@@ -2656,17 +2656,17 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>63</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>65</v>
@@ -2810,58 +2810,58 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B94" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -2882,10 +2882,10 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2898,7 +2898,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>67</v>
@@ -2962,10 +2962,10 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2978,138 +2978,138 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B113" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B113" s="15" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B114" s="15" t="s">
         <v>243</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B115" s="15" t="s">
         <v>228</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" s="15" t="s">
         <v>226</v>
-      </c>
-      <c r="B116" s="15" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B117" s="15" t="s">
         <v>224</v>
-      </c>
-      <c r="B117" s="15" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B118" s="15" t="s">
         <v>230</v>
-      </c>
-      <c r="B118" s="15" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B119" s="15" t="s">
         <v>232</v>
-      </c>
-      <c r="B119" s="15" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="15" t="s">
         <v>245</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B122" s="15" t="s">
         <v>234</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B124" s="15" t="s">
         <v>236</v>
-      </c>
-      <c r="B124" s="15" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B126" s="9" t="s">
         <v>252</v>
-      </c>
-      <c r="B126" s="9" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -3117,7 +3117,7 @@
         <v>9</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -3178,7 +3178,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>74</v>
@@ -3186,15 +3186,15 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B139" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>75</v>
@@ -3202,10 +3202,10 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -3269,15 +3269,15 @@
         <v>16</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -3285,7 +3285,7 @@
         <v>170</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>